<commit_message>
Taller 1, 2, 3 :DONE
</commit_message>
<xml_diff>
--- a/CORTE I/Solver_I/Solver_I.xlsx
+++ b/CORTE I/Solver_I/Solver_I.xlsx
@@ -1,13 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willi\Desktop\GITHUB\OPTIMIZACION_LINEAL\CORTE I\Solver_I\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F762BDAB-88BF-41B6-92F1-BFC54F26FB7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="T5P5" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,9 +24,184 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="42">
+  <si>
+    <t xml:space="preserve">PROBLEMA 5. REFINERÍAS </t>
+  </si>
+  <si>
+    <t>Tres refinerías con capacidades diarias de 6, 5 y 8 millones de galones, respectivamente, abastecen tres áreas de distribución con demandas diarias de 4, 8 y 7 millones de galones, respectivamente. La gasolina se transporta a las tres áreas de distribución a través de una red de oleoductos. El costo de transporte es de 10 centavos por 1000 galones por milla de oleoducto. La Tabla presenta la distancia en millas entre las refinerías y las áreas de distribución. La refinería 1 no está conectada al área de distribución 3.</t>
+  </si>
+  <si>
+    <t>Primal</t>
+  </si>
+  <si>
+    <t>x1</t>
+  </si>
+  <si>
+    <t>x2</t>
+  </si>
+  <si>
+    <t>s1</t>
+  </si>
+  <si>
+    <t>a1</t>
+  </si>
+  <si>
+    <t>s2</t>
+  </si>
+  <si>
+    <t>s3</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>C_B</t>
+  </si>
+  <si>
+    <t>C_N</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Z_max= 600 </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>X1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 800 </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>X2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 0 S1 + 0 S2 + 0S3 - 1000000 A1</t>
+    </r>
+  </si>
+  <si>
+    <t>40 X1 + 50 X2 &gt;= 400</t>
+  </si>
+  <si>
+    <t>X1 + X2 &lt;= 9</t>
+  </si>
+  <si>
+    <t>X1 &lt;= 8</t>
+  </si>
+  <si>
+    <t>X2 &lt;= 10</t>
+  </si>
+  <si>
+    <t>40 X1 + 50 X2  - S1  + A1 = 400</t>
+  </si>
+  <si>
+    <t>X1 + X2 + S2 = 9</t>
+  </si>
+  <si>
+    <t>X1 + S3 = 8</t>
+  </si>
+  <si>
+    <t>MINIMIZAR¡¡</t>
+  </si>
+  <si>
+    <t>X11: Galones enviados de Refineria 1 a Area 1</t>
+  </si>
+  <si>
+    <t>X12: Galones enviados de Refineria 1 a Area 2</t>
+  </si>
+  <si>
+    <t>X13: Galones enviados de Refineria 1 a Area 3</t>
+  </si>
+  <si>
+    <t>X21: Galones enviados de Refineria 2 a Area 1</t>
+  </si>
+  <si>
+    <t>X22: Galones enviados de Refineria 2 a Area 2</t>
+  </si>
+  <si>
+    <t>X23: Galones enviados de Refineria 2 a Area 3</t>
+  </si>
+  <si>
+    <t>X31: Galones enviados de Refineria 3 a Area 1</t>
+  </si>
+  <si>
+    <t>X32: Galones enviados de Refineria 3 a Area 2</t>
+  </si>
+  <si>
+    <t>X33: Galones enviados de Refineria 3 a Area 3</t>
+  </si>
+  <si>
+    <t>Refineria</t>
+  </si>
+  <si>
+    <t>Area de distribucion</t>
+  </si>
+  <si>
+    <t>X11 + X12 = 6</t>
+  </si>
+  <si>
+    <t>X21 + X22 + X23 = 5</t>
+  </si>
+  <si>
+    <t>X31  + X32 + X33 = 8</t>
+  </si>
+  <si>
+    <t>X11 + X21 + X31 = 4</t>
+  </si>
+  <si>
+    <t>X12 + X22 + X32 = 8</t>
+  </si>
+  <si>
+    <t>X13 = 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> X23 + X33 = 7</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,16 +209,47 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -45,12 +257,114 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +644,509 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:T43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="46.44140625" customWidth="1"/>
+    <col min="2" max="2" width="48.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="144" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B3" s="3"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="Q4" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="R4" s="18"/>
+      <c r="S4" s="18"/>
+      <c r="T4" s="18"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B5" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="O5" s="4"/>
+      <c r="Q5" s="19"/>
+      <c r="R5" s="19">
+        <v>1</v>
+      </c>
+      <c r="S5" s="19">
+        <v>2</v>
+      </c>
+      <c r="T5" s="19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="P6" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q6" s="19">
+        <v>1</v>
+      </c>
+      <c r="R6" s="20">
+        <v>100</v>
+      </c>
+      <c r="S6" s="20">
+        <v>180</v>
+      </c>
+      <c r="T6" s="20"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="P7" s="21"/>
+      <c r="Q7" s="19">
+        <v>1</v>
+      </c>
+      <c r="R7" s="20">
+        <v>300</v>
+      </c>
+      <c r="S7" s="20">
+        <v>100</v>
+      </c>
+      <c r="T7" s="20">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B8" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="P8" s="21"/>
+      <c r="Q8" s="19">
+        <v>3</v>
+      </c>
+      <c r="R8" s="20">
+        <v>200</v>
+      </c>
+      <c r="S8" s="20">
+        <v>250</v>
+      </c>
+      <c r="T8" s="20">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B9" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B10" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B11" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B12" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B15" s="22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B16" s="22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B17" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B18" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B19" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B20" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B21" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="K21" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L21" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="M21" s="8"/>
+      <c r="N21" s="4"/>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B22" s="12"/>
+      <c r="C22" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="4"/>
+      <c r="F22" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" s="9">
+        <v>40</v>
+      </c>
+      <c r="H22" s="9">
+        <v>50</v>
+      </c>
+      <c r="I22" s="9">
+        <v>-1</v>
+      </c>
+      <c r="J22" s="9">
+        <v>1</v>
+      </c>
+      <c r="K22" s="9">
+        <v>0</v>
+      </c>
+      <c r="L22" s="9">
+        <v>0</v>
+      </c>
+      <c r="M22" s="10"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="P22" s="11">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B23" s="3"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="9">
+        <v>1</v>
+      </c>
+      <c r="H23" s="9">
+        <v>1</v>
+      </c>
+      <c r="I23" s="9">
+        <v>0</v>
+      </c>
+      <c r="J23" s="9">
+        <v>0</v>
+      </c>
+      <c r="K23" s="9">
+        <v>1</v>
+      </c>
+      <c r="L23" s="9">
+        <v>0</v>
+      </c>
+      <c r="M23" s="10"/>
+      <c r="O23" s="4"/>
+      <c r="P23" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B24" s="3"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24" s="8"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="11">
+        <v>1</v>
+      </c>
+      <c r="H24" s="11">
+        <v>0</v>
+      </c>
+      <c r="I24" s="11">
+        <v>0</v>
+      </c>
+      <c r="J24" s="11">
+        <v>0</v>
+      </c>
+      <c r="K24" s="11">
+        <v>0</v>
+      </c>
+      <c r="L24" s="11">
+        <v>1</v>
+      </c>
+      <c r="M24" s="4"/>
+      <c r="N24" s="4"/>
+      <c r="O24" s="4"/>
+      <c r="P24" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B25" s="13"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
+      <c r="O25" s="4"/>
+    </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B26" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="4"/>
+      <c r="D26" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="4"/>
+      <c r="L26" s="4"/>
+      <c r="N26" s="4"/>
+      <c r="O26" s="4"/>
+    </row>
+    <row r="27" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B27" s="14"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" s="4"/>
+      <c r="F27" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G27" s="11">
+        <v>-600</v>
+      </c>
+      <c r="H27" s="11">
+        <v>-800</v>
+      </c>
+      <c r="I27" s="11">
+        <v>0</v>
+      </c>
+      <c r="J27" s="11">
+        <v>10000</v>
+      </c>
+      <c r="K27" s="11">
+        <v>0</v>
+      </c>
+      <c r="L27" s="11">
+        <v>0</v>
+      </c>
+      <c r="M27" s="4"/>
+      <c r="O27" s="4"/>
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B28" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" s="4"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G28" s="11">
+        <v>10000</v>
+      </c>
+      <c r="H28" s="11">
+        <v>0</v>
+      </c>
+      <c r="I28" s="11">
+        <v>0</v>
+      </c>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="M28" s="4"/>
+      <c r="O28" s="4"/>
+    </row>
+    <row r="29" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B29" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G29" s="11">
+        <v>-600</v>
+      </c>
+      <c r="H29" s="11">
+        <v>-800</v>
+      </c>
+      <c r="I29" s="11">
+        <v>0</v>
+      </c>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+      <c r="O29" s="4"/>
+    </row>
+    <row r="30" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B30" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B31" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B32" s="13"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="17"/>
+      <c r="I32" s="17"/>
+      <c r="J32" s="17"/>
+      <c r="K32" s="17"/>
+      <c r="L32" s="17"/>
+      <c r="M32" s="17"/>
+      <c r="N32" s="17"/>
+    </row>
+    <row r="33" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B33" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="4"/>
+      <c r="K33" s="4"/>
+      <c r="L33" s="4"/>
+      <c r="M33" s="4"/>
+      <c r="N33" s="4"/>
+    </row>
+    <row r="34" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B34" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B35" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B36" s="4"/>
+    </row>
+    <row r="41" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B41" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B42" s="16"/>
+    </row>
+    <row r="43" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B43" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="E19:M19"/>
+    <mergeCell ref="P6:P8"/>
+    <mergeCell ref="Q4:T4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>